<commit_message>
+ tutorial & FMOD begin
</commit_message>
<xml_diff>
--- a/Docs/AudioDuration.xlsx
+++ b/Docs/AudioDuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameDev\Unity\ACASH\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF21A99E-BE99-48E4-B1B8-2EF2C6166B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8230A9AC-3CB1-4477-82E2-6A19DC25DCB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="1260" windowWidth="21960" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="141">
   <si>
     <t>Объяснение фраз</t>
   </si>
@@ -1292,7 +1292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1398,6 +1398,9 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1406,6 +1409,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1440,15 +1449,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1457,6 +1457,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1741,7 +1744,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1753,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1764,7 +1767,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
+      <c r="A2" s="68"/>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1776,7 +1779,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1788,7 +1791,7 @@
       <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1798,7 +1801,7 @@
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1808,7 +1811,7 @@
       <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1818,7 +1821,7 @@
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +1829,7 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1834,7 +1837,7 @@
       <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
@@ -1842,7 +1845,7 @@
       <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="67"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
@@ -1850,7 +1853,7 @@
       <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="67"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1858,7 +1861,7 @@
       <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="68"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1866,7 +1869,7 @@
       <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="72" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1878,7 +1881,7 @@
       <c r="D13" s="30"/>
     </row>
     <row r="14" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="70"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
@@ -1888,7 +1891,7 @@
       <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="70"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="9" t="s">
         <v>32</v>
       </c>
@@ -1898,7 +1901,7 @@
       <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
@@ -1906,7 +1909,7 @@
       <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="10" t="s">
         <v>34</v>
       </c>
@@ -1914,7 +1917,7 @@
       <c r="D17" s="58"/>
     </row>
     <row r="18" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="75" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -1926,7 +1929,7 @@
       <c r="D18" s="59"/>
     </row>
     <row r="19" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="73"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="6" t="s">
         <v>36</v>
       </c>
@@ -1936,7 +1939,7 @@
       <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="73"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
@@ -1946,7 +1949,7 @@
       <c r="D20" s="25"/>
     </row>
     <row r="21" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="73"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
@@ -1954,7 +1957,7 @@
       <c r="D21" s="25"/>
     </row>
     <row r="22" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="12" t="s">
         <v>39</v>
       </c>
@@ -1962,7 +1965,7 @@
       <c r="D22" s="60"/>
     </row>
     <row r="23" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -1974,7 +1977,7 @@
       <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="76"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="16" t="s">
         <v>41</v>
       </c>
@@ -1984,7 +1987,7 @@
       <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="76"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="16" t="s">
         <v>42</v>
       </c>
@@ -1994,7 +1997,7 @@
       <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="19" t="s">
         <v>43</v>
       </c>
@@ -2002,7 +2005,7 @@
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61" t="s">
+      <c r="A27" s="62" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -2014,7 +2017,7 @@
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="62"/>
+      <c r="A28" s="63"/>
       <c r="B28" s="5" t="s">
         <v>45</v>
       </c>
@@ -2024,7 +2027,7 @@
       <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="62"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="5" t="s">
         <v>46</v>
       </c>
@@ -2034,7 +2037,7 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="7" t="s">
         <v>47</v>
       </c>
@@ -2042,7 +2045,7 @@
       <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="65" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="28" t="s">
@@ -2054,7 +2057,7 @@
       <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="76"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="16" t="s">
         <v>49</v>
       </c>
@@ -2064,7 +2067,7 @@
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="19" t="s">
         <v>50</v>
       </c>
@@ -2074,7 +2077,7 @@
       <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="62" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -2086,7 +2089,7 @@
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="62"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="31" t="s">
         <v>52</v>
       </c>
@@ -2096,7 +2099,7 @@
       <c r="D35" s="25"/>
     </row>
     <row r="36" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="63"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="32" t="s">
         <v>53</v>
       </c>
@@ -2106,7 +2109,7 @@
       <c r="D36" s="27"/>
     </row>
     <row r="37" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="75" t="s">
+      <c r="A37" s="65" t="s">
         <v>24</v>
       </c>
       <c r="B37" s="28" t="s">
@@ -2118,7 +2121,7 @@
       <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="76"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="16" t="s">
         <v>55</v>
       </c>
@@ -2128,7 +2131,7 @@
       <c r="D38" s="18"/>
     </row>
     <row r="39" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="76"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="16" t="s">
         <v>56</v>
       </c>
@@ -2138,7 +2141,7 @@
       <c r="D39" s="18"/>
     </row>
     <row r="40" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="76"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="16" t="s">
         <v>57</v>
       </c>
@@ -2146,7 +2149,7 @@
       <c r="D40" s="18"/>
     </row>
     <row r="41" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="76"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="19" t="s">
         <v>58</v>
       </c>
@@ -2154,7 +2157,7 @@
       <c r="D41" s="21"/>
     </row>
     <row r="42" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="61" t="s">
+      <c r="A42" s="62" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -2166,7 +2169,7 @@
       <c r="D42" s="23"/>
     </row>
     <row r="43" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="62"/>
+      <c r="A43" s="63"/>
       <c r="B43" s="5" t="s">
         <v>60</v>
       </c>
@@ -2176,7 +2179,7 @@
       <c r="D43" s="25"/>
     </row>
     <row r="44" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="62"/>
+      <c r="A44" s="63"/>
       <c r="B44" s="5" t="s">
         <v>61</v>
       </c>
@@ -2186,7 +2189,7 @@
       <c r="D44" s="25"/>
     </row>
     <row r="45" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="62"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="5" t="s">
         <v>62</v>
       </c>
@@ -2194,7 +2197,7 @@
       <c r="D45" s="25"/>
     </row>
     <row r="46" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="7" t="s">
         <v>63</v>
       </c>
@@ -2202,7 +2205,7 @@
       <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="76" t="s">
+      <c r="A47" s="61" t="s">
         <v>26</v>
       </c>
       <c r="B47" s="28" t="s">
@@ -2214,7 +2217,7 @@
       <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="76"/>
+      <c r="A48" s="61"/>
       <c r="B48" s="16" t="s">
         <v>65</v>
       </c>
@@ -2224,7 +2227,7 @@
       <c r="D48" s="18"/>
     </row>
     <row r="49" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="76"/>
+      <c r="A49" s="61"/>
       <c r="B49" s="16" t="s">
         <v>74</v>
       </c>
@@ -2234,7 +2237,7 @@
       <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="76"/>
+      <c r="A50" s="61"/>
       <c r="B50" s="19" t="s">
         <v>75</v>
       </c>
@@ -2242,7 +2245,7 @@
       <c r="D50" s="21"/>
     </row>
     <row r="51" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="61" t="s">
+      <c r="A51" s="62" t="s">
         <v>27</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -2254,7 +2257,7 @@
       <c r="D51" s="23"/>
     </row>
     <row r="52" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="62"/>
+      <c r="A52" s="63"/>
       <c r="B52" s="5" t="s">
         <v>77</v>
       </c>
@@ -2264,7 +2267,7 @@
       <c r="D52" s="25"/>
     </row>
     <row r="53" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="62"/>
+      <c r="A53" s="63"/>
       <c r="B53" s="5" t="s">
         <v>66</v>
       </c>
@@ -2274,7 +2277,7 @@
       <c r="D53" s="25"/>
     </row>
     <row r="54" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="63"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="7" t="s">
         <v>67</v>
       </c>
@@ -2282,7 +2285,7 @@
       <c r="D54" s="27"/>
     </row>
     <row r="55" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="76" t="s">
+      <c r="A55" s="61" t="s">
         <v>28</v>
       </c>
       <c r="B55" s="28" t="s">
@@ -2294,7 +2297,7 @@
       <c r="D55" s="30"/>
     </row>
     <row r="56" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="76"/>
+      <c r="A56" s="61"/>
       <c r="B56" s="16" t="s">
         <v>69</v>
       </c>
@@ -2304,7 +2307,7 @@
       <c r="D56" s="18"/>
     </row>
     <row r="57" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="76"/>
+      <c r="A57" s="61"/>
       <c r="B57" s="19" t="s">
         <v>70</v>
       </c>
@@ -2314,7 +2317,7 @@
       <c r="D57" s="21"/>
     </row>
     <row r="58" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="61" t="s">
+      <c r="A58" s="62" t="s">
         <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -2326,7 +2329,7 @@
       <c r="D58" s="23"/>
     </row>
     <row r="59" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="62"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="31" t="s">
         <v>72</v>
       </c>
@@ -2336,7 +2339,7 @@
       <c r="D59" s="25"/>
     </row>
     <row r="60" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="63"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="32" t="s">
         <v>73</v>
       </c>
@@ -2349,7 +2352,7 @@
       <c r="B61" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="81" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2357,7 +2360,7 @@
       <c r="B62" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2365,7 +2368,7 @@
       <c r="B63" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="81" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2373,7 +2376,7 @@
       <c r="B64" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2381,7 +2384,7 @@
       <c r="B65" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="81" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2389,7 +2392,7 @@
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2397,15 +2400,15 @@
       <c r="B67" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="1">
-        <v>2</v>
+      <c r="C67" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2413,15 +2416,15 @@
       <c r="B69" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C69" s="1">
-        <v>2</v>
+      <c r="C69" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2429,15 +2432,15 @@
       <c r="B71" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C71" s="1">
-        <v>2</v>
+      <c r="C71" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2445,15 +2448,15 @@
       <c r="B73" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C73" s="1">
-        <v>2</v>
+      <c r="C73" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2461,15 +2464,15 @@
       <c r="B75" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="1">
-        <v>2</v>
+      <c r="C75" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2477,15 +2480,15 @@
       <c r="B77" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C77" s="1">
-        <v>2</v>
+      <c r="C77" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="81" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2493,7 +2496,7 @@
       <c r="B79" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="81" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2501,7 +2504,7 @@
       <c r="B80" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="81" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2509,7 +2512,7 @@
       <c r="B81" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="81" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3434,6 +3437,12 @@
     <row r="1000" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A55:A57"/>
     <mergeCell ref="A58:A60"/>
     <mergeCell ref="A31:A33"/>
@@ -3442,12 +3451,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -3469,7 +3472,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="67" t="s">
         <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3525,7 +3528,7 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
+      <c r="A2" s="68"/>
       <c r="B2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3555,7 +3558,7 @@
       <c r="X2" s="80"/>
     </row>
     <row r="3" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="69" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3570,7 +3573,7 @@
       <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="5" t="s">
         <v>81</v>
       </c>
@@ -3582,7 +3585,7 @@
       <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="5" t="s">
         <v>82</v>
       </c>
@@ -3594,7 +3597,7 @@
       <c r="F5" s="45"/>
     </row>
     <row r="6" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="5" t="s">
         <v>83</v>
       </c>
@@ -3606,7 +3609,7 @@
       <c r="F6" s="45"/>
     </row>
     <row r="7" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="5" t="s">
         <v>84</v>
       </c>
@@ -3618,7 +3621,7 @@
       <c r="F7" s="45"/>
     </row>
     <row r="8" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="5" t="s">
         <v>85</v>
       </c>
@@ -3630,7 +3633,7 @@
       <c r="F8" s="45"/>
     </row>
     <row r="9" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="5" t="s">
         <v>127</v>
       </c>
@@ -3642,7 +3645,7 @@
       <c r="F9" s="45"/>
     </row>
     <row r="10" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="67"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="5" t="s">
         <v>128</v>
       </c>
@@ -3654,7 +3657,7 @@
       <c r="F10" s="45"/>
     </row>
     <row r="11" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="67"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="5" t="s">
         <v>86</v>
       </c>
@@ -3666,7 +3669,7 @@
       <c r="F11" s="45"/>
     </row>
     <row r="12" spans="1:24" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="68"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="7" t="s">
         <v>87</v>
       </c>
@@ -3678,7 +3681,7 @@
       <c r="F12" s="45"/>
     </row>
     <row r="13" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="8" t="s">
         <v>88</v>
       </c>
@@ -3690,7 +3693,7 @@
       <c r="F13" s="45"/>
     </row>
     <row r="14" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="70"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="9" t="s">
         <v>89</v>
       </c>
@@ -3702,7 +3705,7 @@
       <c r="F14" s="50"/>
     </row>
     <row r="15" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="70"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="9" t="s">
         <v>90</v>
       </c>
@@ -3714,7 +3717,7 @@
       <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="9" t="s">
         <v>91</v>
       </c>
@@ -3726,7 +3729,7 @@
       <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:6" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="10" t="s">
         <v>92</v>
       </c>

</xml_diff>